<commit_message>
V0.3 de Especificación de Requerimientos V0.7 de SRS V1.4 de SPMP
</commit_message>
<xml_diff>
--- a/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/Actas de Monitoreo de Desarrollo/(SnoutPoint) - Monitoreo de Desarrollo de Documento - SRS - Req Especificos.xlsx
+++ b/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/Actas de Monitoreo de Desarrollo/(SnoutPoint) - Monitoreo de Desarrollo de Documento - SRS - Req Especificos.xlsx
@@ -298,9 +298,6 @@
     <t>Se explica el contenido aplicado de la plantilla de Requerimientos específicos</t>
   </si>
   <si>
-    <t>v0.6</t>
-  </si>
-  <si>
     <t>22 de Abril de 2015</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>Si, tiene las clasificación de requerimientos y ejemplos del excel de los requerimientos específicos.</t>
+  </si>
+  <si>
+    <t>v0.7</t>
   </si>
 </sst>
 </file>
@@ -454,6 +454,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,36 +495,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,7 +768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -779,337 +779,318 @@
   <dimension ref="B1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D10" sqref="D10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="5" width="11.42578125" style="16"/>
-    <col min="6" max="6" width="13.7109375" style="16" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="4"/>
+    <col min="6" max="6" width="13.7109375" style="4" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="2:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="2:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="2:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="2:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B17:F35"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="B1:F2"/>
@@ -1118,6 +1099,25 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B17:F35"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>